<commit_message>
Initial Performer implementation: queue processing, summary email, system exception handling
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\C#\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MorisMwaiWachira\OneDrive - THH LLC\Documents\UiPath\T2G_EmailSummaryBot\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEA6D7A-A5A1-4970-A74B-0D350BFA0880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2505" yWindow="-13740" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="57">
   <si>
     <t>Name</t>
   </si>
@@ -88,10 +88,6 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -161,6 +157,59 @@
   </si>
   <si>
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>FilteredEmailsQueue</t>
+  </si>
+  <si>
+    <t>T2G_EmailAutomation</t>
+  </si>
+  <si>
+    <t>SystemExEmailSubject</t>
+  </si>
+  <si>
+    <t>Automation error!</t>
+  </si>
+  <si>
+    <t>SummaryEmailSubject</t>
+  </si>
+  <si>
+    <t>Email Automation Summary</t>
+  </si>
+  <si>
+    <t>SummaryEmailBody</t>
+  </si>
+  <si>
+    <t>SummaryNotificationEmail</t>
+  </si>
+  <si>
+    <t>ExceptionNotificationEmail</t>
+  </si>
+  <si>
+    <t>SystemExEmailBody</t>
+  </si>
+  <si>
+    <t>Hello, 
+An exception occurred during the automation process.  Please find the details below:
+Exception Source: @Source
+Exception Message: @Message
+A screenshot of the error has been attached for reference. Please see the attachment for more details.
+Thank you and have a good day,
+T2G Automation Bot :)</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Hello,
+The automation successfully processed:
+- Partnership/Investor Emails: @ProcessedEmails
+- CV Emails with Attachments: @ProcessedWithAttachments
+Timestamp: @Timestamp
+Note: All processed emails have been moved to the 'Processed Mails' folder.
+Attachments (if any) are saved in the Dispatcher's output folder: Data/Output/Attachments.
+Best regards,  
+T2G Automation Bot :)</t>
   </si>
 </sst>
 </file>
@@ -212,21 +261,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -245,9 +289,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -285,7 +329,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -391,7 +435,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -533,7 +577,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -543,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -591,25 +635,28 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="7" t="s">
-        <v>38</v>
+      <c r="A3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="7"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
@@ -619,7 +666,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -631,10 +678,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z17"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -687,24 +734,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
@@ -725,7 +770,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -747,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -758,7 +803,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -769,56 +814,83 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="5">
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="5" t="s">
+      <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="5">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="17" spans="1:3" ht="45">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>40</v>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="240">
+      <c r="A21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="195">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -832,7 +904,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -851,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -879,9 +951,30 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>